<commit_message>
kicad: Fix resistor value on remote
</commit_message>
<xml_diff>
--- a/kicad/remote/remote-bom.xlsx
+++ b/kicad/remote/remote-bom.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -252,6 +252,24 @@
   </si>
   <si>
     <t>TQFP-32</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>LED (any color)</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>330 Ohm</t>
   </si>
 </sst>
 </file>
@@ -441,7 +459,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -518,9 +536,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -748,9 +763,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -830,7 +845,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -857,10 +872,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1107,9 +1122,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1387,7 +1402,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1414,10 +1429,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1659,7 +1674,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1668,7 +1683,7 @@
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.8984" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.8516" style="1" customWidth="1"/>
     <col min="5" max="5" width="23.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="45" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.5" style="1" customWidth="1"/>
@@ -2006,6 +2021,52 @@
         <v>14</v>
       </c>
       <c r="I16" s="3"/>
+    </row>
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="A17" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="C17" s="23">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="G17" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="H17" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="A18" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="C18" s="23">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="G18" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="H18" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="I18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2034,74 +2095,74 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.45" customHeight="1">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="14.45" customHeight="1">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" ht="14.45" customHeight="1">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" ht="14.45" customHeight="1">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" ht="14.45" customHeight="1">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" ht="14.45" customHeight="1">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" ht="14.45" customHeight="1">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" ht="14.45" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" ht="14.45" customHeight="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" ht="14.45" customHeight="1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.699306" right="0.699306" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2120,79 +2181,79 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="6" style="27" customWidth="1"/>
-    <col min="6" max="16384" width="6" style="27" customWidth="1"/>
+    <col min="1" max="5" width="6" style="26" customWidth="1"/>
+    <col min="6" max="16384" width="6" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.45" customHeight="1">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="14.45" customHeight="1">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" ht="14.45" customHeight="1">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" ht="14.45" customHeight="1">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" ht="14.45" customHeight="1">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" ht="14.45" customHeight="1">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" ht="14.45" customHeight="1">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" ht="14.45" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" ht="14.45" customHeight="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" ht="14.45" customHeight="1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.699306" right="0.699306" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>